<commit_message>
1. added picture with named rectangles 2. added colors
</commit_message>
<xml_diff>
--- a/SMPTETestPattern/smpte.xlsx
+++ b/SMPTETestPattern/smpte.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Height</t>
   </si>
@@ -28,6 +28,63 @@
   </si>
   <si>
     <t>%Width</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>0xff696969</t>
+  </si>
+  <si>
+    <t>c1c1c1</t>
+  </si>
+  <si>
+    <t>c1c100</t>
+  </si>
+  <si>
+    <t>00c1c1</t>
+  </si>
+  <si>
+    <t>00c100</t>
+  </si>
+  <si>
+    <t>c100c1</t>
+  </si>
+  <si>
+    <t>c10000</t>
+  </si>
+  <si>
+    <t>0000c1</t>
+  </si>
+  <si>
+    <t>00ffff</t>
+  </si>
+  <si>
+    <t>0000ff</t>
+  </si>
+  <si>
+    <t>ffff00</t>
+  </si>
+  <si>
+    <t>36056d</t>
+  </si>
+  <si>
+    <t>fdfdfd</t>
+  </si>
+  <si>
+    <t>ff0000</t>
+  </si>
+  <si>
+    <t>2b2b2b</t>
+  </si>
+  <si>
+    <t>ffffff</t>
+  </si>
+  <si>
+    <t>0a0a0a</t>
+  </si>
+  <si>
+    <t>0d0d0d</t>
   </si>
 </sst>
 </file>
@@ -66,9 +123,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,18 +423,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5">
+    <row r="1" spans="2:7">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -387,16 +448,22 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="2:5">
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7">
       <c r="B2">
         <v>504</v>
       </c>
       <c r="C2">
         <v>896</v>
       </c>
-    </row>
-    <row r="3" spans="2:5">
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
       <c r="B3">
         <v>294</v>
       </c>
@@ -411,8 +478,11 @@
         <f>C3/$C$2</f>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="4" spans="2:5">
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
       <c r="B4">
         <v>294</v>
       </c>
@@ -420,15 +490,18 @@
         <v>96</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D15" si="0">B4/$B$2</f>
+        <f t="shared" ref="D4:D13" si="0">B4/$B$2</f>
         <v>0.58333333333333337</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E15" si="1">C4/$C$2</f>
+        <f t="shared" ref="E4:E13" si="1">C4/$C$2</f>
         <v>0.10714285714285714</v>
       </c>
-    </row>
-    <row r="5" spans="2:5">
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
       <c r="B5">
         <v>42</v>
       </c>
@@ -443,8 +516,11 @@
         <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="6" spans="2:5">
+      <c r="G5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
       <c r="C6">
         <v>576</v>
       </c>
@@ -456,8 +532,11 @@
         <f t="shared" si="1"/>
         <v>0.6428571428571429</v>
       </c>
-    </row>
-    <row r="7" spans="2:5">
+      <c r="G6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
       <c r="B7">
         <v>126</v>
       </c>
@@ -472,8 +551,11 @@
         <f>C7/$C$2</f>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="G7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
       <c r="B8">
         <v>126</v>
       </c>
@@ -488,8 +570,11 @@
         <f t="shared" si="1"/>
         <v>0.1875</v>
       </c>
-    </row>
-    <row r="9" spans="2:5">
+      <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
       <c r="B9">
         <v>126</v>
       </c>
@@ -504,8 +589,11 @@
         <f t="shared" si="1"/>
         <v>0.21875</v>
       </c>
-    </row>
-    <row r="10" spans="2:5">
+      <c r="G9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
       <c r="C10">
         <v>90</v>
       </c>
@@ -517,8 +605,11 @@
         <f t="shared" si="1"/>
         <v>0.10044642857142858</v>
       </c>
-    </row>
-    <row r="11" spans="2:5">
+      <c r="G10" s="2">
+        <v>696969</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
       <c r="C11">
         <v>30</v>
       </c>
@@ -530,8 +621,11 @@
         <f t="shared" si="1"/>
         <v>3.3482142857142856E-2</v>
       </c>
-    </row>
-    <row r="12" spans="2:5">
+      <c r="G11" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
       <c r="C12">
         <v>96</v>
       </c>
@@ -543,8 +637,11 @@
         <f t="shared" si="1"/>
         <v>0.10714285714285714</v>
       </c>
-    </row>
-    <row r="13" spans="2:5">
+      <c r="G12" s="2">
+        <v>52550</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
       <c r="C13">
         <v>112</v>
       </c>
@@ -556,14 +653,96 @@
         <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="14" spans="2:5">
+      <c r="G13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="2:5">
+      <c r="G14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
+      <c r="G15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="G16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8">
+      <c r="G17" s="2">
+        <v>50505</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8">
+      <c r="G19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8">
+      <c r="G20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8">
+      <c r="G21" s="2">
+        <v>50505</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8">
+      <c r="G22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="7:8">
+      <c r="G23" s="2">
+        <v>50505</v>
+      </c>
+    </row>
+    <row r="24" spans="7:8">
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="7:8">
+      <c r="G25" s="2">
+        <v>50505</v>
+      </c>
+    </row>
+    <row r="26" spans="7:8">
+      <c r="G26" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="7:8">
+      <c r="G27" s="2">
+        <v>50505</v>
+      </c>
+    </row>
+    <row r="28" spans="7:8">
+      <c r="G28" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="7:8">
+      <c r="G29" s="2">
+        <v>50505</v>
+      </c>
+    </row>
+    <row r="30" spans="7:8">
+      <c r="G30" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>